<commit_message>
Adicionando base de dados da Mega-Sena
</commit_message>
<xml_diff>
--- a/MegaSena.xlsx
+++ b/MegaSena.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7530" tabRatio="876"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7530" tabRatio="876"/>
   </bookViews>
   <sheets>
     <sheet name="MEGA SENA" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2956" uniqueCount="2956">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2962" uniqueCount="2962">
   <si>
     <t>Concurso</t>
   </si>
@@ -8892,6 +8892,24 @@
   </si>
   <si>
     <t>06/12/2025</t>
+  </si>
+  <si>
+    <t>09/12/2025</t>
+  </si>
+  <si>
+    <t>11/12/2025</t>
+  </si>
+  <si>
+    <t>13/12/2025</t>
+  </si>
+  <si>
+    <t>16/12/2025</t>
+  </si>
+  <si>
+    <t>18/12/2025</t>
+  </si>
+  <si>
+    <t>20/12/2025</t>
   </si>
 </sst>
 </file>
@@ -9278,10 +9296,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2949"/>
+  <dimension ref="A1:H2955"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2931" workbookViewId="0">
-      <selection activeCell="H2952" sqref="H2952"/>
+    <sheetView tabSelected="1" topLeftCell="A2940" workbookViewId="0">
+      <selection activeCell="E2960" sqref="E2960"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -85966,6 +85984,162 @@
       </c>
       <c r="H2949">
         <v>53</v>
+      </c>
+    </row>
+    <row r="2950" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2950">
+        <v>2949</v>
+      </c>
+      <c r="B2950" t="s">
+        <v>2956</v>
+      </c>
+      <c r="C2950">
+        <v>6</v>
+      </c>
+      <c r="D2950">
+        <v>11</v>
+      </c>
+      <c r="E2950">
+        <v>4</v>
+      </c>
+      <c r="F2950">
+        <v>49</v>
+      </c>
+      <c r="G2950">
+        <v>54</v>
+      </c>
+      <c r="H2950">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2951" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2951">
+        <v>2950</v>
+      </c>
+      <c r="B2951" t="s">
+        <v>2957</v>
+      </c>
+      <c r="C2951">
+        <v>21</v>
+      </c>
+      <c r="D2951">
+        <v>42</v>
+      </c>
+      <c r="E2951">
+        <v>50</v>
+      </c>
+      <c r="F2951">
+        <v>23</v>
+      </c>
+      <c r="G2951">
+        <v>49</v>
+      </c>
+      <c r="H2951">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2952" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2952">
+        <v>2951</v>
+      </c>
+      <c r="B2952" t="s">
+        <v>2958</v>
+      </c>
+      <c r="C2952">
+        <v>8</v>
+      </c>
+      <c r="D2952">
+        <v>31</v>
+      </c>
+      <c r="E2952">
+        <v>37</v>
+      </c>
+      <c r="F2952">
+        <v>30</v>
+      </c>
+      <c r="G2952">
+        <v>45</v>
+      </c>
+      <c r="H2952">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2953" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2953">
+        <v>2952</v>
+      </c>
+      <c r="B2953" t="s">
+        <v>2959</v>
+      </c>
+      <c r="C2953">
+        <v>45</v>
+      </c>
+      <c r="D2953">
+        <v>51</v>
+      </c>
+      <c r="E2953">
+        <v>20</v>
+      </c>
+      <c r="F2953">
+        <v>48</v>
+      </c>
+      <c r="G2953">
+        <v>1</v>
+      </c>
+      <c r="H2953">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2954" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2954">
+        <v>2953</v>
+      </c>
+      <c r="B2954" t="s">
+        <v>2960</v>
+      </c>
+      <c r="C2954">
+        <v>54</v>
+      </c>
+      <c r="D2954">
+        <v>24</v>
+      </c>
+      <c r="E2954">
+        <v>47</v>
+      </c>
+      <c r="F2954">
+        <v>25</v>
+      </c>
+      <c r="G2954">
+        <v>10</v>
+      </c>
+      <c r="H2954">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2955" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2955">
+        <v>2954</v>
+      </c>
+      <c r="B2955" t="s">
+        <v>2961</v>
+      </c>
+      <c r="C2955">
+        <v>37</v>
+      </c>
+      <c r="D2955">
+        <v>1</v>
+      </c>
+      <c r="E2955">
+        <v>42</v>
+      </c>
+      <c r="F2955">
+        <v>44</v>
+      </c>
+      <c r="G2955">
+        <v>39</v>
+      </c>
+      <c r="H2955">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -85984,16 +86158,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <AtualizadoPeloTimerJobEm xmlns="4455b8ba-124f-46d5-aaaa-9813efd83d1e">2025-11-23T04:12:54+00:00</AtualizadoPeloTimerJobEm>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C92CDE8829F3C7438DCCB0991C30EAAE" ma:contentTypeVersion="3" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="36cf41eecaf38ba1d849a0c8dd067090">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="3e38fcf2-aa96-4a2c-865b-c3abba01ba51" xmlns:ns3="4455b8ba-124f-46d5-aaaa-9813efd83d1e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="023f68b2d27389a617bf935a3f0e17ad" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -86161,6 +86325,16 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <AtualizadoPeloTimerJobEm xmlns="4455b8ba-124f-46d5-aaaa-9813efd83d1e">2025-11-23T04:12:54+00:00</AtualizadoPeloTimerJobEm>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{834FBCC7-87B2-49AB-8978-479962E2FF95}">
   <ds:schemaRefs>
@@ -86170,17 +86344,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64615F65-CF13-4100-B135-FA0CB5E1C951}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="4455b8ba-124f-46d5-aaaa-9813efd83d1e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9445F805-6E3A-4841-AEBD-CF7F6CDA924D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -86198,4 +86361,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64615F65-CF13-4100-B135-FA0CB5E1C951}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="4455b8ba-124f-46d5-aaaa-9813efd83d1e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>